<commit_message>
review expected results 200
</commit_message>
<xml_diff>
--- a/mobile-subscribersoffers-v1.xlsx
+++ b/mobile-subscribersoffers-v1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="172">
   <si>
     <t>Subject</t>
   </si>
@@ -54,13 +54,201 @@
     <t>mobile-subscribersoffers-v1</t>
   </si>
   <si>
-    <t>CT001.01 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+    <t>CT001.01 - Request enviada com sucesso - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Ok - COD 200</t>
   </si>
   <si>
     <t xml:space="preserve">Operação responsável por Adição de ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - AdicionarOfertasAssinantesv1
 APIGEE
 POST
 https://api-test.claro.com.br/mobile/v1/subscribers/offers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "serviceType": "MOVEL",
+  "subscriptionType": "CLARO_CARTAO",
+  "telephoneNumber": "1191000000",
+  "id": "123456"
+}</t>
+  </si>
+  <si>
+    <t>Z415515</t>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+{
+  "data": {
+    "subscriber": {
+      "serviceType": "MOVEL",
+      "subscriptionType": "CLARO_CARTAO",
+      "device": {
+        "telephoneNumber": "1191000000"
+      },
+      "offers": [
+        {
+          "id": "123456"
+        }
+      ]
+    }
+  }
+}
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Busca apresenta sucesso.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "data": {
+    "subscriber": {
+      "serviceType": "MOVEL",
+      "subscriptionType": "CLARO_CARTAO",
+      "device": {
+        "telephoneNumber": "1191000000"
+      },
+      "offers": [
+        {
+          "id": "123456"
+        }
+      ]
+    }
+  }
+}
+APIGEE = 200</t>
+  </si>
+  <si>
+    <t>MANUAL</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Hitss</t>
+  </si>
+  <si>
+    <t>Novo</t>
+  </si>
+  <si>
+    <t>CT001.02 - Request enviada com sucesso - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Ok - COD 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "id": 123456,
+  "serviceType": "MOVEL",
+  "subscriptionType": "CLARO_CONTA",
+  "offersType": {
+    "id": 123456
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+{
+  "data": {
+    "subscriber": {
+      "id": 123456,
+      "serviceType": "MOVEL",
+      "subscriptionType": "CLARO_CONTA",
+      "salesman": {
+        "id": "123456",
+        "salesAgent": {
+          "id": "123456"
+        }
+      },
+      "offers": [
+        {
+          "id": 123456,
+          "level": "CONTRATO",
+          "startDate": "2009-01-01",
+          "endDate": "2010-03-01",
+          "isSubsidy": false,
+          "subsidyValue": "CONTRATO",
+          "parameters": [
+            {
+              "name": "JOAO DA SILVA",
+              "values": [
+                {
+                  "value": "z01"
+                }
+              ]
+            }
+          ]
+        }
+      ]
+    }
+  }
+}
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Busca apresenta sucesso.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "data": {
+    "subscriber": {
+      "id": 123456,
+      "serviceType": "MOVEL",
+      "subscriptionType": "CLARO_CONTA",
+      "offers": [
+        {
+          "id": 123456,
+          "level": "CONTRATO",
+          "startDate": "2009-01-01",
+          "endDate": "2010-03-01",
+          "name": "Sigilo do Número do Originador",
+          "category": {
+            "id": "SIGILO"
+          }
+        }
+      ]
+    }
+  }
+}
+APIGEE = 200</t>
+  </si>
+  <si>
+    <t>CT001.03 - Request enviada com sucesso - Interface-Adicionar-Ofertas-Assinante-Common-Category - Ok - COD 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "telephoneNumber": "11910000",
+  "partyType": "PF",
+  "subscriptionType": "CLARO_CONTROLE",
+  "commonCategory": "BLOQUEIO_TOTAL_DADOS"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+{
+  "data": {
+    "telephoneNumber": "11910000",
+    "mobileSubscriberId": "308586112",
+    "partyType": "PF",
+    "subscriptionType": "CLARO_CONTROLE",
+    "commonCategory": "BLOQUEIO_TOTAL_DADOS"
+  }
+}
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Busca apresenta sucesso.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2023-05-22",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac"
+}
+APIGEE = 200</t>
+  </si>
+  <si>
+    <t>CT002.01 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -69,12 +257,6 @@
   "telephoneNumber": 1191000000,
   "id": "SIGILO"
 }</t>
-  </si>
-  <si>
-    <t>Z415515</t>
-  </si>
-  <si>
-    <t>Step 1</t>
   </si>
   <si>
     <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
@@ -91,37 +273,23 @@
     <t xml:space="preserve">1 - Busca apresenta falha.
 2 - Response retorna os seguintes valores:
 {
-  "value": {
-    "apiVersion": "1;2021-08-17",
-    "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
-    "error": {
-      "httpCode": "400",
-      "errorCode": "API-SUBSCRIBERSOFFERS-400",
-      "message": "Bad Request",
-      "detailedMessage": "Invalid Request for operation.",
-      "link": {
-        "rel": "related",
-        "href": "https://api.claro.com.br/docs"
-      }
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "401",
+    "errorCode": "API-SUBSCRIBERSOFFERS-401",
+    "message": "Unauthorized",
+    "detailedMessage": "Unauthorized user.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
     }
   }
 }
-APIGEE = 400</t>
-  </si>
-  <si>
-    <t>MANUAL</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Hitss</t>
-  </si>
-  <si>
-    <t>Novo</t>
-  </si>
-  <si>
-    <t>CT001.02 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+APIGEE = 401</t>
+  </si>
+  <si>
+    <t>CT002.02 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -143,7 +311,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.03 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "403",
+    "errorCode": "API-SUBSCRIBERSOFFERS-403",
+    "message": "Forbidden",
+    "detailedMessage": "Access denied.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 403</t>
+  </si>
+  <si>
+    <t>CT002.03 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -165,7 +352,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.04 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "404",
+    "errorCode": "API-SUBSCRIBERSOFFERS-404",
+    "message": "Not found",
+    "detailedMessage": "Resource not found.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 404</t>
+  </si>
+  <si>
+    <t>CT002.04 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -187,7 +393,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.05 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "405",
+    "errorCode": "API-SUBSCRIBERSOFFERS-405",
+    "message": "Method Not Allowed",
+    "detailedMessage": "Unavailable HTTP method.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 405</t>
+  </si>
+  <si>
+    <t>CT002.05 - Request enviada com falha - Interface1-Adicionar-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -209,7 +434,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.06 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "406",
+    "errorCode": "API-SUBSCRIBERSOFFERS-406",
+    "message": "Request Not Acceptable",
+    "detailedMessage": "Requested content type not acceptable.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 406</t>
+  </si>
+  <si>
+    <t>CT002.06 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -235,7 +479,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.07 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "415",
+    "errorCode": "API-SUBSCRIBERSOFFERS-415",
+    "message": "Unsupported Media Type",
+    "detailedMessage": "Unsupported request media type.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 415</t>
+  </si>
+  <si>
+    <t>CT002.07 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -261,7 +524,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.08 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "429",
+    "errorCode": "API-SUBSCRIBERSOFFERS-429",
+    "message": "Too Many Requests",
+    "detailedMessage": "Consumer requests exceeded policies.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 429</t>
+  </si>
+  <si>
+    <t>CT002.08 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -287,7 +569,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.09 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "400",
+    "errorCode": "API-SUBSCRIBERSOFFERS-001",
+    "message": "Bad Request",
+    "detailedMessage": "O campo [nome_campo] é obrigatório.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 400</t>
+  </si>
+  <si>
+    <t>CT002.09 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -309,7 +610,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.10 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t>CT002.10 - Request enviada com falha - Interface3-Adicionar-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -331,7 +632,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.11 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+    <t>CT002.11 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -353,7 +654,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.12 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+    <t>CT002.12 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -375,7 +676,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.13 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+    <t>CT002.13 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -397,7 +698,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.14 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+    <t>CT002.14 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -419,7 +720,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.15 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+    <t>CT002.15 - Request enviada com falha - Interface-Adicionar-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -441,7 +742,113 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.01 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+    <t>CT003 - Request enviada com falha - Unauthorized - COD 401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authorization: ' ' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+Authorization: ' ' 
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 401</t>
+  </si>
+  <si>
+    <t>CT004 - Request enviada com falha - Forbidden - COD 403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por Adição de ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - AdicionarOfertasAssinantesv1
+APIGEE
+POST
+https://api-test.claro.com.br/mobile/v1/(.*)/subscribers/offers</t>
+  </si>
+  <si>
+    <t>https://api-test.claro.com.br/mobile/v1/(.*)/subscribers/offers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+https://api-test.claro.com.br/mobile/v1/(.*)/subscribers/offers
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 403</t>
+  </si>
+  <si>
+    <t>CT005 - Request enviada com falha - Not Found - COD 404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por Adição de ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - AdicionarOfertasAssinantesv1
+APIGEE
+POST
+https://api-test.claro.com.br/mobile/v1/subscribers/offers/smart</t>
+  </si>
+  <si>
+    <t>https://api-test.claro.com.br/mobile/v1/subscribers/offers/smart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+https://api-test.claro.com.br/mobile/v1/subscribers/offers/smart
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 404</t>
+  </si>
+  <si>
+    <t>CT006 - Request enviada com falha - Method Not Allowed - COD 405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por Adição de ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - AdicionarOfertasAssinantesv1
+APIGEE
+PATCH
+https://api-test.claro.com.br/mobile/v1/subscribers/offers</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+PATCH
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 405</t>
+  </si>
+  <si>
+    <t>CT007 - Request enviada com falha - Not Acceptable - COD 406</t>
+  </si>
+  <si>
+    <t>Accept: text/plain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+Accept: text/plain
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 406</t>
+  </si>
+  <si>
+    <t>CT008 - Request enviada com falha - Unsupported Media Type - COD 415</t>
+  </si>
+  <si>
+    <t>Content-Type: text/plain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+Content-Type: text/plain
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 415</t>
+  </si>
+  <si>
+    <t>CT009 - Request enviada com falha - Too Many Requests - COD 429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://api-test.claro.com.br/mobile/v1/subscribers/offers
+https://api-test.claro.com.br/mobile/v1/subscribers/offers
+https://api-test.claro.com.br/mobile/v1/subscribers/offers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+https://api-test.claro.com.br/mobile/v1/subscribers/offers
+https://api-test.claro.com.br/mobile/v1/subscribers/offers
+https://api-test.claro.com.br/mobile/v1/subscribers/offers
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 429</t>
+  </si>
+  <si>
+    <t>CT001.01 - Request enviada com sucesso - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Ok - COD 200</t>
   </si>
   <si>
     <t xml:space="preserve">Operação responsável por Remover as ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - RemoverOfertasAssinantesv1
@@ -450,19 +857,55 @@
 https://api-test.claro.com.br/mobile/v1/subscribers/offers</t>
   </si>
   <si>
-    <t>CT001.02 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.03 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.04 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.05 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.06 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t>CT001.02 - Request enviada com sucesso - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Ok - COD 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+  "id": 123456,
+  "serviceType": "MOVEL",
+  "subscriptionType": "CLARO_CONTA"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - Para validação do request, execute a API com os seguintes parâmetros:
+{
+  "data": {
+    "subscriber": {
+      "id": 123456,
+      "serviceType": "MOVEL",
+      "subscriptionType": "CLARO_CONTA",
+      "offers": [
+        {
+          "id": 321456456,
+          "level": "CONTRATO"
+        }
+      ]
+    }
+  }
+}
+2 - O response retornado deve apresentar o seguinte valor:
+APIGEE = 200</t>
+  </si>
+  <si>
+    <t>CT001.03 - Request enviada com sucesso - Interface-Remover-Ofertas-Assinante-Common-Category - Ok - COD 200</t>
+  </si>
+  <si>
+    <t>CT002.01 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.02 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.03 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.04 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.05 - Request enviada com falha - Interface1-Remover-Ofertas-Assinante-PrePago-Codigo-Oferta - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.06 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -482,7 +925,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.07 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t>CT002.07 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -502,7 +945,7 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.08 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t>CT002.08 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -522,7 +965,26 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.09 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
+    <t xml:space="preserve">1 - Busca apresenta falha.
+2 - Response retorna os seguintes valores:
+{
+  "apiVersion": "1;2021-08-17",
+  "transactionId": "d86cebae-779d-4255-a479-1c0dd912dfac",
+  "error": {
+    "httpCode": "400",
+    "errorCode": "API-SUBSCRIBERSOFFERS-006",
+    "message": "Bad Request",
+    "detailedMessage": "O campo [nome_campo] é obrigatório.",
+    "link": {
+      "rel": "related",
+      "href": "https://api.claro.com.br/docs"
+    }
+  }
+}
+APIGEE = 400</t>
+  </si>
+  <si>
+    <t>CT002.09 - Request enviada com falha - Interface3-Remover-Ofertas-Assinante-PosPago-Controle-Codigo-Oferta - Bad Request - COD 400</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -542,19 +1004,37 @@
 APIGEE = 400</t>
   </si>
   <si>
-    <t>CT001.10 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.11 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.12 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.13 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
-  </si>
-  <si>
-    <t>CT001.14 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+    <t>CT002.10 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.11 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.12 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.13 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t>CT002.14 - Request enviada com falha - Interface-Remover-Ofertas-Assinante-Common-Category - Bad Request - COD 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por Remover as ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - RemoverOfertasAssinantesv1
+APIGEE
+DELETE
+https://api-test.claro.com.br/mobile/v1/(.*)/subscribers/offers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por Remover as ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - RemoverOfertasAssinantesv1
+APIGEE
+DELETE
+https://api-test.claro.com.br/mobile/v1/subscribers/offers/smart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por Remover as ofertas para um assinante pós/control ou pré-pago. Backend: SOA Móvel - RemoverOfertasAssinantesv1
+APIGEE
+PATCH
+https://api-test.claro.com.br/mobile/v1/subscribers/offers</t>
   </si>
   <si>
     <t>CT001.01 - Request enviada com falha - Bad Request - COD 400</t>
@@ -695,6 +1175,51 @@
 }
 2 - O response retornado deve apresentar o seguinte valor:
 APIGEE = 400</t>
+  </si>
+  <si>
+    <t>CT002 - Request enviada com falha - Unauthorized - COD 401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por listar as ofertas de um assinante pós, controle ou pré-pago. Backend: SOA Móvel
+APIGEE
+GET
+https://api-test.claro.com.br/mobile/v1/subscribers/offers</t>
+  </si>
+  <si>
+    <t>CT003 - Request enviada com falha - Forbidden - COD 403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por listar as ofertas de um assinante pós, controle ou pré-pago. Backend: SOA Móvel
+APIGEE
+GET
+https://api-test.claro.com.br/mobile/v1/(.*)/subscribers/offers</t>
+  </si>
+  <si>
+    <t>CT004 - Request enviada com falha - Not Found - COD 404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por listar as ofertas de um assinante pós, controle ou pré-pago. Backend: SOA Móvel
+APIGEE
+GET
+https://api-test.claro.com.br/mobile/v1/subscribers/offers/smart</t>
+  </si>
+  <si>
+    <t>CT005 - Request enviada com falha - Method Not Allowed - COD 405</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operação responsável por listar as ofertas de um assinante pós, controle ou pré-pago. Backend: SOA Móvel
+APIGEE
+PATCH
+https://api-test.claro.com.br/mobile/v1/subscribers/offers</t>
+  </si>
+  <si>
+    <t>CT006 - Request enviada com falha - Not Acceptable - COD 406</t>
+  </si>
+  <si>
+    <t>CT007 - Request enviada com falha - Unsupported Media Type - COD 415</t>
+  </si>
+  <si>
+    <t>CT008 - Request enviada com falha - Too Many Requests - COD 429</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1613,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
@@ -1200,7 +1725,7 @@
         <v>26</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>20</v>
@@ -1220,13 +1745,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1235,10 +1760,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>20</v>
@@ -1258,13 +1783,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -1273,10 +1798,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>20</v>
@@ -1296,13 +1821,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
@@ -1311,10 +1836,10 @@
         <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>20</v>
@@ -1334,13 +1859,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
@@ -1349,10 +1874,10 @@
         <v>17</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>20</v>
@@ -1372,13 +1897,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>16</v>
@@ -1387,10 +1912,10 @@
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>20</v>
@@ -1410,13 +1935,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
@@ -1425,10 +1950,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>20</v>
@@ -1448,13 +1973,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>16</v>
@@ -1463,10 +1988,10 @@
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>20</v>
@@ -1486,13 +2011,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>16</v>
@@ -1501,10 +2026,10 @@
         <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>20</v>
@@ -1524,13 +2049,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>16</v>
@@ -1539,10 +2064,10 @@
         <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>20</v>
@@ -1562,13 +2087,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
@@ -1577,10 +2102,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>20</v>
@@ -1600,13 +2125,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
@@ -1615,10 +2140,10 @@
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>20</v>
@@ -1638,13 +2163,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>16</v>
@@ -1653,10 +2178,10 @@
         <v>17</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>20</v>
@@ -1676,13 +2201,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>16</v>
@@ -1691,10 +2216,10 @@
         <v>17</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>20</v>
@@ -1706,6 +2231,386 @@
         <v>22</v>
       </c>
       <c r="L16" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1717,7 +2622,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L25"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
@@ -1773,10 +2678,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>15</v>
@@ -1811,13 +2716,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
@@ -1826,10 +2731,10 @@
         <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>20</v>
@@ -1849,13 +2754,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -1864,10 +2769,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>20</v>
@@ -1887,13 +2792,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -1902,10 +2807,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>20</v>
@@ -1925,13 +2830,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>71</v>
+        <v>116</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
@@ -1940,10 +2845,10 @@
         <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>20</v>
@@ -1963,13 +2868,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
@@ -1978,10 +2883,10 @@
         <v>17</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>20</v>
@@ -2001,13 +2906,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>16</v>
@@ -2016,10 +2921,10 @@
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>20</v>
@@ -2039,13 +2944,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
@@ -2054,10 +2959,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>20</v>
@@ -2077,13 +2982,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>16</v>
@@ -2092,10 +2997,10 @@
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>20</v>
@@ -2115,13 +3020,13 @@
         <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>16</v>
@@ -2130,10 +3035,10 @@
         <v>17</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>20</v>
@@ -2153,13 +3058,13 @@
         <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>16</v>
@@ -2168,10 +3073,10 @@
         <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>20</v>
@@ -2191,13 +3096,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>86</v>
+        <v>130</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>58</v>
+        <v>131</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>16</v>
@@ -2206,10 +3111,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>59</v>
+        <v>132</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>20</v>
@@ -2229,13 +3134,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>67</v>
+        <v>110</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>16</v>
@@ -2244,10 +3149,10 @@
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>20</v>
@@ -2267,36 +3172,416 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="2" t="s">
+      <c r="C20" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2308,11 +3593,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="62" customWidth="1"/>
+    <col min="2" max="2" width="70" customWidth="1"/>
     <col min="3" max="4" width="102" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
@@ -2365,13 +3650,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>16</v>
@@ -2380,10 +3665,10 @@
         <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>20</v>
@@ -2403,13 +3688,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
@@ -2418,10 +3703,10 @@
         <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>20</v>
@@ -2441,13 +3726,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>16</v>
@@ -2456,10 +3741,10 @@
         <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>20</v>
@@ -2479,13 +3764,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -2494,10 +3779,10 @@
         <v>17</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>104</v>
+        <v>156</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>20</v>
@@ -2517,36 +3802,302 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="H12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" ht="50" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="E13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="H13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>